<commit_message>
Bug fixes. Resolved compatibility issues.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
   <si>
     <t>Course Title</t>
   </si>
@@ -44,10 +44,11 @@
     <t>39 total hours</t>
   </si>
   <si>
-    <t>4.7</t>
-  </si>
-  <si>
-    <t>(15,495 ratings)</t>
+    <t>Rating: 4.7 out of 5
+4.7</t>
+  </si>
+  <si>
+    <t>(15,792)</t>
   </si>
   <si>
     <t>Build an app with ASPNET Core and Angular from scratch</t>
@@ -62,10 +63,11 @@
     <t>29 total hours</t>
   </si>
   <si>
-    <t>4.6</t>
-  </si>
-  <si>
-    <t>(10,481 ratings)</t>
+    <t>Rating: 4.6 out of 5
+4.6</t>
+  </si>
+  <si>
+    <t>(10,820)</t>
   </si>
   <si>
     <t>ES6 Javascript: The Complete Developer's Guide</t>
@@ -80,16 +82,17 @@
     <t>6 total hours</t>
   </si>
   <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>(8,457 ratings)</t>
+    <t>Rating: 4.5 out of 5
+4.5</t>
+  </si>
+  <si>
+    <t>(8,532)</t>
   </si>
   <si>
     <t>Beginner Full Stack Web Development: HTML, CSS, React &amp; Node</t>
   </si>
   <si>
-    <t>Mark Price</t>
+    <t>Mark Price, Devslopes by Mark Price</t>
   </si>
   <si>
     <t>159 lectures</t>
@@ -98,10 +101,11 @@
     <t>30 total hours</t>
   </si>
   <si>
-    <t>4.4</t>
-  </si>
-  <si>
-    <t>(7,771 ratings)</t>
+    <t>Rating: 4.4 out of 5
+4.4</t>
+  </si>
+  <si>
+    <t>(7,933)</t>
   </si>
   <si>
     <t>Git a Web Developer Job: Mastering the Modern Workflow</t>
@@ -113,13 +117,17 @@
     <t>15 total hours</t>
   </si>
   <si>
-    <t>(5,611 ratings)</t>
+    <t>Rating: 4.8 out of 5
+4.8</t>
+  </si>
+  <si>
+    <t>(5,700)</t>
   </si>
   <si>
     <t>Build Websites from Scratch with HTML &amp; CSS</t>
   </si>
   <si>
-    <t>Brad Hussey</t>
+    <t>Brad Hussey, Code College</t>
   </si>
   <si>
     <t>77 lectures</t>
@@ -128,7 +136,7 @@
     <t>8 total hours</t>
   </si>
   <si>
-    <t>(5,046 ratings)</t>
+    <t>(5,187)</t>
   </si>
   <si>
     <t>JavaScript Beginner Bootcamp (2020)</t>
@@ -137,13 +145,13 @@
     <t>Rob Merrill</t>
   </si>
   <si>
-    <t>384 lectures</t>
+    <t>386 lectures</t>
   </si>
   <si>
     <t>38.5 total hours</t>
   </si>
   <si>
-    <t>(4,643 ratings)</t>
+    <t>(4,709)</t>
   </si>
   <si>
     <t>Django 2.2 &amp; Python | The Ultimate Web Development Bootcamp</t>
@@ -158,7 +166,7 @@
     <t>10 total hours</t>
   </si>
   <si>
-    <t>(4,366 ratings)</t>
+    <t>(4,468)</t>
   </si>
   <si>
     <t>The Modern React Bootcamp (Hooks, Context, NextJS, Router)</t>
@@ -170,13 +178,28 @@
     <t>312 lectures</t>
   </si>
   <si>
-    <t>(3,264 ratings)</t>
+    <t>(3,433)</t>
   </si>
   <si>
     <t>Electron for Desktop Apps: The Complete Developer's Guide</t>
   </si>
   <si>
-    <t>(2,434 ratings)</t>
+    <t>(2,477)</t>
+  </si>
+  <si>
+    <t>Build a Backend REST API with Python &amp; Django - Beginner</t>
+  </si>
+  <si>
+    <t>Mark Winterbottom, Brooke Rutherford</t>
+  </si>
+  <si>
+    <t>76 lectures</t>
+  </si>
+  <si>
+    <t>5 total hours</t>
+  </si>
+  <si>
+    <t>(2,363)</t>
   </si>
   <si>
     <t>Docker for Developers and DevOps</t>
@@ -191,85 +214,11 @@
     <t>5.5 total hours</t>
   </si>
   <si>
-    <t>3.9</t>
-  </si>
-  <si>
-    <t>(2,314 ratings)</t>
-  </si>
-  <si>
-    <t>Build a Backend REST API with Python &amp; Django - Beginner</t>
-  </si>
-  <si>
-    <t>Mark Winterbottom</t>
-  </si>
-  <si>
-    <t>76 lectures</t>
-  </si>
-  <si>
-    <t>5 total hours</t>
-  </si>
-  <si>
-    <t>(2,266 ratings)</t>
-  </si>
-  <si>
-    <t>The Full Stack Web Development</t>
-  </si>
-  <si>
-    <t>Eduonix Learning Solutions</t>
-  </si>
-  <si>
-    <t>208 lectures</t>
-  </si>
-  <si>
-    <t>33 total hours</t>
-  </si>
-  <si>
-    <t>(2,223 ratings)</t>
-  </si>
-  <si>
-    <t>Learn PHP Fundamentals From Scratch</t>
-  </si>
-  <si>
-    <t>10 lectures</t>
-  </si>
-  <si>
-    <t>2 total hours</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>(2,183 ratings)</t>
-  </si>
-  <si>
-    <t>React JS, Angular &amp; Vue JS - Quickstart &amp; Comparison</t>
-  </si>
-  <si>
-    <t>Maximilian Schwarzmüller</t>
-  </si>
-  <si>
-    <t>144 lectures</t>
-  </si>
-  <si>
-    <t>(2,041 ratings)</t>
-  </si>
-  <si>
-    <t>Front End Web Development For Beginners (A Practical Guide)</t>
-  </si>
-  <si>
-    <t>Learn Tech Plus</t>
-  </si>
-  <si>
-    <t>31 lectures</t>
-  </si>
-  <si>
-    <t>3.5 total hours</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>(1,895 ratings)</t>
+    <t>Rating: 3.8 out of 5
+3.8</t>
+  </si>
+  <si>
+    <t>(2,322)</t>
   </si>
 </sst>
 </file>
@@ -314,7 +263,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -434,81 +383,81 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -517,44 +466,44 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
         <v>60</v>
@@ -574,90 +523,10 @@
         <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>